<commit_message>
Updated to reflect that multiple sprites can be on one tile.
</commit_message>
<xml_diff>
--- a/docs/move-decision.xlsx
+++ b/docs/move-decision.xlsx
@@ -1,36 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23117"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="13395" windowHeight="5415"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24340" windowHeight="15480"/>
   </bookViews>
   <sheets>
-    <sheet name="decision-table" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="FilledIn" sheetId="1" r:id="rId1"/>
+    <sheet name="empty" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>Conditions</t>
   </si>
   <si>
-    <t>Mover</t>
-  </si>
-  <si>
     <t>Ghost</t>
   </si>
   <si>
     <t>Player</t>
-  </si>
-  <si>
-    <t>Target Tile</t>
   </si>
   <si>
     <t>Empty</t>
@@ -99,13 +99,31 @@
   <si>
     <t>move poss.;
 food remains</t>
+  </si>
+  <si>
+    <t>Mover = …</t>
+  </si>
+  <si>
+    <t>Action:</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>move possible;</t>
+  </si>
+  <si>
+    <t>Move possible means that the mover becomes the new top most sprite at the target tile.</t>
+  </si>
+  <si>
+    <t>Topmost Target Tile = …</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +135,35 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -164,24 +211,91 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -190,14 +304,39 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -489,198 +628,265 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="6" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="17"/>
+      <c r="B3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="19"/>
+      <c r="B5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="19"/>
+      <c r="B6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="19"/>
+      <c r="B7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" thickBot="1">
+      <c r="A8" s="20"/>
+      <c r="B8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="42" customHeight="1">
+      <c r="A9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="6"/>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="7"/>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="7"/>
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="7"/>
-      <c r="B7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="7"/>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="42" customHeight="1">
-      <c r="A9" s="2" t="s">
+      <c r="I9" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="4" t="s">
+      <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="B13" t="s">
+      <c r="B14" s="15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -689,30 +895,205 @@
     <mergeCell ref="A4:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="17"/>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="19"/>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="19"/>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="19"/>
+      <c r="B7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1">
+      <c r="A8" s="20"/>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" ht="42" customHeight="1">
+      <c r="A9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="D12" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>